<commit_message>
Added reports folder and a new dump
</commit_message>
<xml_diff>
--- a/Integrated Project/Gauteng MMS/web/Reports/Monthly/Audit Trail/2013-June Report - Audit Trail.xlsx
+++ b/Integrated Project/Gauteng MMS/web/Reports/Monthly/Audit Trail/2013-June Report - Audit Trail.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="34">
   <si>
     <t>Forensic Pathology Service</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Event Message</t>
   </si>
   <si>
-    <t>2013-05-21</t>
+    <t>2013-06-03</t>
   </si>
   <si>
     <t>Log In</t>
@@ -44,25 +44,10 @@
     <t>Log In Screen</t>
   </si>
   <si>
-    <t>Successfull log in</t>
-  </si>
-  <si>
-    <t>2013-05-20</t>
-  </si>
-  <si>
     <t>User2</t>
   </si>
   <si>
-    <t>2013-05-22</t>
-  </si>
-  <si>
-    <t>2013-05-23</t>
-  </si>
-  <si>
-    <t>2013-05-24</t>
-  </si>
-  <si>
-    <t>2013-06-03</t>
+    <t>Successfull log in</t>
   </si>
   <si>
     <t>Warning</t>
@@ -81,6 +66,54 @@
   </si>
   <si>
     <t>Created new incident 00120130604</t>
+  </si>
+  <si>
+    <t>2013-06-05</t>
+  </si>
+  <si>
+    <t>2013-06-07</t>
+  </si>
+  <si>
+    <t>Closed Incident</t>
+  </si>
+  <si>
+    <t>Open Incidents Tab</t>
+  </si>
+  <si>
+    <t>Closed incident 002201301</t>
+  </si>
+  <si>
+    <t>Closed incident 00120130604</t>
+  </si>
+  <si>
+    <t>Created new incident 00120130607</t>
+  </si>
+  <si>
+    <t>Dispatch Vehicle</t>
+  </si>
+  <si>
+    <t>Dispatched vehicle ABC123GP</t>
+  </si>
+  <si>
+    <t>Incident has been edited</t>
+  </si>
+  <si>
+    <t>Edit Incident Details Tab</t>
+  </si>
+  <si>
+    <t>Incident details of incident 00120130607 has been edited</t>
+  </si>
+  <si>
+    <t>2013-06-09</t>
+  </si>
+  <si>
+    <t>2013-06-10</t>
+  </si>
+  <si>
+    <t>2013-06-11</t>
+  </si>
+  <si>
+    <t>2013-06-13</t>
   </si>
 </sst>
 </file>
@@ -349,7 +382,7 @@
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6" t="n" s="1">
-        <v>41435.461930439815</v>
+        <v>41439.324962453706</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -461,11 +494,11 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -475,7 +508,7 @@
     </row>
     <row r="13" ht="30.0" customHeight="true">
       <c r="A13" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
@@ -487,11 +520,11 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -501,7 +534,7 @@
     </row>
     <row r="14" ht="30.0" customHeight="true">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
@@ -513,11 +546,11 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -527,7 +560,7 @@
     </row>
     <row r="15" ht="30.0" customHeight="true">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
@@ -539,11 +572,11 @@
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -553,7 +586,7 @@
     </row>
     <row r="16" ht="30.0" customHeight="true">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -565,11 +598,11 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -579,7 +612,7 @@
     </row>
     <row r="17" ht="30.0" customHeight="true">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -591,11 +624,11 @@
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -605,7 +638,7 @@
     </row>
     <row r="18" ht="30.0" customHeight="true">
       <c r="A18" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -617,11 +650,11 @@
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -643,11 +676,11 @@
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -669,11 +702,11 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -695,11 +728,11 @@
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -709,7 +742,7 @@
     </row>
     <row r="22" ht="30.0" customHeight="true">
       <c r="A22" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
@@ -721,11 +754,11 @@
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -735,7 +768,7 @@
     </row>
     <row r="23" ht="30.0" customHeight="true">
       <c r="A23" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
@@ -747,11 +780,11 @@
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -761,7 +794,7 @@
     </row>
     <row r="24" ht="30.0" customHeight="true">
       <c r="A24" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
@@ -773,11 +806,11 @@
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -787,11 +820,11 @@
     </row>
     <row r="25" ht="30.0" customHeight="true">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
@@ -799,11 +832,11 @@
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -813,7 +846,7 @@
     </row>
     <row r="26" ht="30.0" customHeight="true">
       <c r="A26" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -825,11 +858,11 @@
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -839,7 +872,7 @@
     </row>
     <row r="27" ht="30.0" customHeight="true">
       <c r="A27" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
@@ -851,11 +884,11 @@
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -865,7 +898,7 @@
     </row>
     <row r="28" ht="30.0" customHeight="true">
       <c r="A28" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
@@ -877,11 +910,11 @@
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -891,7 +924,7 @@
     </row>
     <row r="29" ht="30.0" customHeight="true">
       <c r="A29" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
@@ -903,11 +936,11 @@
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -917,7 +950,7 @@
     </row>
     <row r="30" ht="30.0" customHeight="true">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
@@ -929,11 +962,11 @@
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -943,7 +976,7 @@
     </row>
     <row r="31" ht="30.0" customHeight="true">
       <c r="A31" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
@@ -955,11 +988,11 @@
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -969,7 +1002,7 @@
     </row>
     <row r="32" ht="30.0" customHeight="true">
       <c r="A32" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5" t="s">
@@ -981,11 +1014,11 @@
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -995,7 +1028,7 @@
     </row>
     <row r="33" ht="30.0" customHeight="true">
       <c r="A33" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
@@ -1007,11 +1040,11 @@
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1021,7 +1054,7 @@
     </row>
     <row r="34" ht="30.0" customHeight="true">
       <c r="A34" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -1033,11 +1066,11 @@
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -1047,7 +1080,7 @@
     </row>
     <row r="35" ht="30.0" customHeight="true">
       <c r="A35" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
@@ -1059,11 +1092,11 @@
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -1073,7 +1106,7 @@
     </row>
     <row r="36" ht="30.0" customHeight="true">
       <c r="A36" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
@@ -1085,11 +1118,11 @@
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -1099,7 +1132,7 @@
     </row>
     <row r="37" ht="30.0" customHeight="true">
       <c r="A37" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
@@ -1111,11 +1144,11 @@
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -1125,23 +1158,23 @@
     </row>
     <row r="38" ht="30.0" customHeight="true">
       <c r="A38" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
@@ -1151,7 +1184,7 @@
     </row>
     <row r="39" ht="30.0" customHeight="true">
       <c r="A39" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
@@ -1163,11 +1196,11 @@
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
@@ -1177,7 +1210,7 @@
     </row>
     <row r="40" ht="30.0" customHeight="true">
       <c r="A40" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
@@ -1189,11 +1222,11 @@
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -1203,7 +1236,7 @@
     </row>
     <row r="41" ht="30.0" customHeight="true">
       <c r="A41" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
@@ -1215,11 +1248,11 @@
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -1229,7 +1262,7 @@
     </row>
     <row r="42" ht="30.0" customHeight="true">
       <c r="A42" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -1241,11 +1274,11 @@
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -1255,7 +1288,7 @@
     </row>
     <row r="43" ht="30.0" customHeight="true">
       <c r="A43" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
@@ -1267,11 +1300,11 @@
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
@@ -1281,7 +1314,7 @@
     </row>
     <row r="44" ht="30.0" customHeight="true">
       <c r="A44" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
@@ -1293,11 +1326,11 @@
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -1307,7 +1340,7 @@
     </row>
     <row r="45" ht="30.0" customHeight="true">
       <c r="A45" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
@@ -1319,11 +1352,11 @@
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
@@ -1333,11 +1366,11 @@
     </row>
     <row r="46" ht="30.0" customHeight="true">
       <c r="A46" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
@@ -1345,11 +1378,11 @@
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
@@ -1359,7 +1392,7 @@
     </row>
     <row r="47" ht="30.0" customHeight="true">
       <c r="A47" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
@@ -1371,11 +1404,11 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
@@ -1385,7 +1418,7 @@
     </row>
     <row r="48" ht="30.0" customHeight="true">
       <c r="A48" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
@@ -1397,11 +1430,11 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
@@ -1411,7 +1444,7 @@
     </row>
     <row r="49" ht="30.0" customHeight="true">
       <c r="A49" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
@@ -1423,11 +1456,11 @@
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
@@ -1437,7 +1470,7 @@
     </row>
     <row r="50" ht="30.0" customHeight="true">
       <c r="A50" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
@@ -1449,11 +1482,11 @@
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
@@ -1463,7 +1496,7 @@
     </row>
     <row r="51" ht="30.0" customHeight="true">
       <c r="A51" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
@@ -1475,11 +1508,11 @@
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -1489,7 +1522,7 @@
     </row>
     <row r="52" ht="30.0" customHeight="true">
       <c r="A52" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
@@ -1501,11 +1534,11 @@
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -1515,7 +1548,7 @@
     </row>
     <row r="53" ht="30.0" customHeight="true">
       <c r="A53" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
@@ -1527,11 +1560,11 @@
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -1541,11 +1574,11 @@
     </row>
     <row r="54" ht="30.0" customHeight="true">
       <c r="A54" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
@@ -1553,11 +1586,11 @@
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
@@ -1567,7 +1600,7 @@
     </row>
     <row r="55" ht="30.0" customHeight="true">
       <c r="A55" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
@@ -1579,11 +1612,11 @@
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
@@ -1593,11 +1626,11 @@
     </row>
     <row r="56" ht="30.0" customHeight="true">
       <c r="A56" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
@@ -1605,11 +1638,11 @@
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
@@ -1619,11 +1652,11 @@
     </row>
     <row r="57" ht="30.0" customHeight="true">
       <c r="A57" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
@@ -1631,11 +1664,11 @@
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -1657,11 +1690,11 @@
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
@@ -1683,7 +1716,7 @@
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
@@ -1701,19 +1734,19 @@
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
@@ -1727,19 +1760,19 @@
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
@@ -1753,19 +1786,19 @@
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
@@ -1774,52 +1807,1014 @@
       <c r="N62" s="5"/>
     </row>
     <row r="63" ht="30.0" customHeight="true">
-      <c r="A63" s="5"/>
+      <c r="A63" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="G63" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="I63" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" ht="15.0" customHeight="true">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-    </row>
-    <row r="65" ht="15.0" customHeight="true">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-      <c r="J65"/>
-      <c r="K65"/>
-      <c r="L65"/>
-      <c r="M65"/>
-      <c r="N65"/>
+    <row r="64" ht="30.0" customHeight="true">
+      <c r="A64" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+    </row>
+    <row r="65" ht="30.0" customHeight="true">
+      <c r="A65" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+    </row>
+    <row r="66" ht="30.0" customHeight="true">
+      <c r="A66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+    </row>
+    <row r="67" ht="30.0" customHeight="true">
+      <c r="A67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+    </row>
+    <row r="68" ht="30.0" customHeight="true">
+      <c r="A68" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" ht="30.0" customHeight="true">
+      <c r="A69" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+    </row>
+    <row r="70" ht="30.0" customHeight="true">
+      <c r="A70" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+    </row>
+    <row r="71" ht="30.0" customHeight="true">
+      <c r="A71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+    </row>
+    <row r="72" ht="30.0" customHeight="true">
+      <c r="A72" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5"/>
+    </row>
+    <row r="73" ht="30.0" customHeight="true">
+      <c r="A73" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+    </row>
+    <row r="74" ht="30.0" customHeight="true">
+      <c r="A74" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+    </row>
+    <row r="75" ht="30.0" customHeight="true">
+      <c r="A75" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+    </row>
+    <row r="76" ht="30.0" customHeight="true">
+      <c r="A76" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+    </row>
+    <row r="77" ht="30.0" customHeight="true">
+      <c r="A77" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+    </row>
+    <row r="78" ht="30.0" customHeight="true">
+      <c r="A78" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+    </row>
+    <row r="79" ht="30.0" customHeight="true">
+      <c r="A79" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+    </row>
+    <row r="80" ht="30.0" customHeight="true">
+      <c r="A80" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+    </row>
+    <row r="81" ht="30.0" customHeight="true">
+      <c r="A81" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+    </row>
+    <row r="82" ht="30.0" customHeight="true">
+      <c r="A82" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+    </row>
+    <row r="83" ht="30.0" customHeight="true">
+      <c r="A83" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+    </row>
+    <row r="84" ht="30.0" customHeight="true">
+      <c r="A84" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+    </row>
+    <row r="85" ht="30.0" customHeight="true">
+      <c r="A85" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+    </row>
+    <row r="86" ht="30.0" customHeight="true">
+      <c r="A86" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+    </row>
+    <row r="87" ht="30.0" customHeight="true">
+      <c r="A87" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+    </row>
+    <row r="88" ht="30.0" customHeight="true">
+      <c r="A88" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+    </row>
+    <row r="89" ht="30.0" customHeight="true">
+      <c r="A89" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+    </row>
+    <row r="90" ht="30.0" customHeight="true">
+      <c r="A90" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+    </row>
+    <row r="91" ht="30.0" customHeight="true">
+      <c r="A91" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+    </row>
+    <row r="92" ht="30.0" customHeight="true">
+      <c r="A92" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+    </row>
+    <row r="93" ht="30.0" customHeight="true">
+      <c r="A93" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+    </row>
+    <row r="94" ht="30.0" customHeight="true">
+      <c r="A94" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+    </row>
+    <row r="95" ht="30.0" customHeight="true">
+      <c r="A95" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+    </row>
+    <row r="96" ht="30.0" customHeight="true">
+      <c r="A96" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+    </row>
+    <row r="97" ht="30.0" customHeight="true">
+      <c r="A97" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+    </row>
+    <row r="98" ht="30.0" customHeight="true">
+      <c r="A98" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+    </row>
+    <row r="99" ht="30.0" customHeight="true">
+      <c r="A99" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
+    </row>
+    <row r="100" ht="30.0" customHeight="true">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+    </row>
+    <row r="101" ht="15.0" customHeight="true">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+    </row>
+    <row r="102" ht="15.0" customHeight="true">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102"/>
+      <c r="M102"/>
+      <c r="N102"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -2194,6 +3189,265 @@
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="K63:L63"/>
     <mergeCell ref="M63:N63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="M76:N76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="M77:N77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="K79:L79"/>
+    <mergeCell ref="M79:N79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="K80:L80"/>
+    <mergeCell ref="M80:N80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="M81:N81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="K82:L82"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="K83:L83"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="K86:L86"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="K88:L88"/>
+    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="K89:L89"/>
+    <mergeCell ref="M89:N89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="K91:L91"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="K92:L92"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="I93:J93"/>
+    <mergeCell ref="K93:L93"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="K94:L94"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="K95:L95"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="K96:L96"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="K97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="K98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="I99:J99"/>
+    <mergeCell ref="K99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="M100:N100"/>
     <mergeCell ref="A1:F6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="K5:N5"/>

</xml_diff>